<commit_message>
practice work of html,css and javascript
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\practice\practice work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\practice\practice work\practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>S_No</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>modal form using html,css and js</t>
+  </si>
+  <si>
+    <t>upload form to practice repo</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +502,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -527,19 +530,19 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -547,126 +550,92 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F10" t="s">
         <v>29</v>
       </c>
+    </row>
+    <row r="11" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1">
         <v>44320</v>
@@ -674,30 +643,11 @@
       <c r="C12" t="s">
         <v>33</v>
       </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
-      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FF0070C0"/>
-          <x14:colorNegative rgb="FF000000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FF000000"/>
-          <x14:colorFirst rgb="FF000000"/>
-          <x14:colorLast rgb="FF000000"/>
-          <x14:colorHigh rgb="FF000000"/>
-          <x14:colorLow rgb="FF000000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!A1:A1</xm:f>
-              <xm:sqref>A11</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-      </x14:sparklineGroups>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>